<commit_message>
Adaptation tool in devlp
</commit_message>
<xml_diff>
--- a/resources/public/tools/current_vulnerability.xlsx
+++ b/resources/public/tools/current_vulnerability.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Current Weather</t>
   </si>
@@ -37,12 +37,6 @@
     <t>Climate Variable</t>
   </si>
   <si>
-    <t>Consequences</t>
-  </si>
-  <si>
-    <t>Thresholds</t>
-  </si>
-  <si>
     <t>Impact</t>
   </si>
   <si>
@@ -107,6 +101,18 @@
   </si>
   <si>
     <t>Record your objectives:</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Exposures</t>
+  </si>
+  <si>
+    <t>Level of Exposure</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
   </si>
 </sst>
 </file>
@@ -323,16 +329,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -623,17 +629,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +665,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,7 +673,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,12 +681,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -692,10 +698,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,76 +721,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="3" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="16"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -792,45 +799,53 @@
         <v>2</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="J11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -838,9 +853,11 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -848,9 +865,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -858,9 +877,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -868,9 +889,11 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -878,9 +901,11 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -888,9 +913,11 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -898,9 +925,11 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -908,9 +937,11 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -918,9 +949,11 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -928,9 +961,11 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -938,9 +973,11 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -948,9 +985,11 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -958,9 +997,11 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -968,9 +1009,11 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -978,9 +1021,11 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -988,9 +1033,11 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -998,9 +1045,11 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1008,9 +1057,11 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1018,9 +1069,11 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1028,9 +1081,11 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1038,9 +1093,11 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1048,9 +1105,11 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1058,9 +1117,11 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1068,9 +1129,11 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1078,9 +1141,11 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1088,9 +1153,11 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1098,9 +1165,11 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1108,9 +1177,11 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1118,9 +1189,11 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1128,9 +1201,11 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1138,9 +1213,11 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1148,9 +1225,11 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1158,9 +1237,11 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1168,9 +1249,11 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1178,13 +1261,15 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="6"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>